<commit_message>
fictitious N numbers for testing
</commit_message>
<xml_diff>
--- a/publication/part1000/CR_itemshape_1/WG_Number_excel_table.xlsx
+++ b/publication/part1000/CR_itemshape_1/WG_Number_excel_table.xlsx
@@ -5,7 +5,7 @@
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/klt/Projets/EclipseWS_CR_itemshape1/stepmod/publication/part1000/CR_itemshape_1/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/klt/Projets/EclipseWS/stepmod/publication/part1000/CR_itemshape_1/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="69">
   <si>
     <t>Kevin Le Tutour</t>
   </si>
@@ -132,6 +132,108 @@
   </si>
   <si>
     <t>ISO 10303-1816 ed2 model_based_3d_geometrical_dimensioning_and_tolerancing_representation ARM EXPRESS</t>
+  </si>
+  <si>
+    <t>N1111</t>
+  </si>
+  <si>
+    <t>N1112</t>
+  </si>
+  <si>
+    <t>N1113</t>
+  </si>
+  <si>
+    <t>N1114</t>
+  </si>
+  <si>
+    <t>N1115</t>
+  </si>
+  <si>
+    <t>N1116</t>
+  </si>
+  <si>
+    <t>N1117</t>
+  </si>
+  <si>
+    <t>N1118</t>
+  </si>
+  <si>
+    <t>N1119</t>
+  </si>
+  <si>
+    <t>N1120</t>
+  </si>
+  <si>
+    <t>N1121</t>
+  </si>
+  <si>
+    <t>N1122</t>
+  </si>
+  <si>
+    <t>N1123</t>
+  </si>
+  <si>
+    <t>N1124</t>
+  </si>
+  <si>
+    <t>N1125</t>
+  </si>
+  <si>
+    <t>N1126</t>
+  </si>
+  <si>
+    <t>N1127</t>
+  </si>
+  <si>
+    <t>N1128</t>
+  </si>
+  <si>
+    <t>N1129</t>
+  </si>
+  <si>
+    <t>N1130</t>
+  </si>
+  <si>
+    <t>N1131</t>
+  </si>
+  <si>
+    <t>N1132</t>
+  </si>
+  <si>
+    <t>N1133</t>
+  </si>
+  <si>
+    <t>N1134</t>
+  </si>
+  <si>
+    <t>N1135</t>
+  </si>
+  <si>
+    <t>N1136</t>
+  </si>
+  <si>
+    <t>N1137</t>
+  </si>
+  <si>
+    <t>N1138</t>
+  </si>
+  <si>
+    <t>N1139</t>
+  </si>
+  <si>
+    <t>N1140</t>
+  </si>
+  <si>
+    <t>N1141</t>
+  </si>
+  <si>
+    <t>N1142</t>
+  </si>
+  <si>
+    <t>N1143</t>
+  </si>
+  <si>
+    <t>N1144</t>
   </si>
 </sst>
 </file>
@@ -480,7 +582,7 @@
   <dimension ref="A1:F34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -492,7 +594,9 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="2"/>
+      <c r="A1" s="2" t="s">
+        <v>35</v>
+      </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
@@ -506,7 +610,9 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="2"/>
+      <c r="A2" s="2" t="s">
+        <v>36</v>
+      </c>
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
@@ -520,7 +626,9 @@
       </c>
     </row>
     <row r="3" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="2"/>
+      <c r="A3" s="2" t="s">
+        <v>37</v>
+      </c>
       <c r="B3" s="2" t="s">
         <v>0</v>
       </c>
@@ -534,7 +642,9 @@
       </c>
     </row>
     <row r="4" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="2"/>
+      <c r="A4" s="2" t="s">
+        <v>38</v>
+      </c>
       <c r="B4" s="2" t="s">
         <v>0</v>
       </c>
@@ -548,7 +658,9 @@
       </c>
     </row>
     <row r="5" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="2"/>
+      <c r="A5" s="2" t="s">
+        <v>39</v>
+      </c>
       <c r="B5" s="2" t="s">
         <v>0</v>
       </c>
@@ -562,7 +674,9 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="2"/>
+      <c r="A6" s="2" t="s">
+        <v>40</v>
+      </c>
       <c r="B6" s="2" t="s">
         <v>0</v>
       </c>
@@ -576,7 +690,9 @@
       </c>
     </row>
     <row r="7" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="2"/>
+      <c r="A7" s="2" t="s">
+        <v>41</v>
+      </c>
       <c r="B7" s="2" t="s">
         <v>0</v>
       </c>
@@ -590,7 +706,9 @@
       </c>
     </row>
     <row r="8" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="2"/>
+      <c r="A8" s="2" t="s">
+        <v>42</v>
+      </c>
       <c r="B8" s="2" t="s">
         <v>0</v>
       </c>
@@ -604,7 +722,9 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="2"/>
+      <c r="A9" s="2" t="s">
+        <v>43</v>
+      </c>
       <c r="B9" s="2" t="s">
         <v>0</v>
       </c>
@@ -618,7 +738,9 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="2"/>
+      <c r="A10" s="2" t="s">
+        <v>44</v>
+      </c>
       <c r="B10" s="2" t="s">
         <v>0</v>
       </c>
@@ -632,7 +754,9 @@
       </c>
     </row>
     <row r="11" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="2"/>
+      <c r="A11" s="2" t="s">
+        <v>45</v>
+      </c>
       <c r="B11" s="2" t="s">
         <v>0</v>
       </c>
@@ -646,7 +770,9 @@
       </c>
     </row>
     <row r="12" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="2"/>
+      <c r="A12" s="2" t="s">
+        <v>46</v>
+      </c>
       <c r="B12" s="2" t="s">
         <v>0</v>
       </c>
@@ -660,7 +786,9 @@
       </c>
     </row>
     <row r="13" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="2"/>
+      <c r="A13" s="2" t="s">
+        <v>47</v>
+      </c>
       <c r="B13" s="2" t="s">
         <v>0</v>
       </c>
@@ -674,7 +802,9 @@
       </c>
     </row>
     <row r="14" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="2"/>
+      <c r="A14" s="2" t="s">
+        <v>48</v>
+      </c>
       <c r="B14" s="2" t="s">
         <v>0</v>
       </c>
@@ -688,7 +818,9 @@
       </c>
     </row>
     <row r="15" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="2"/>
+      <c r="A15" s="2" t="s">
+        <v>49</v>
+      </c>
       <c r="B15" s="2" t="s">
         <v>0</v>
       </c>
@@ -702,7 +834,9 @@
       </c>
     </row>
     <row r="16" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="2"/>
+      <c r="A16" s="2" t="s">
+        <v>50</v>
+      </c>
       <c r="B16" s="2" t="s">
         <v>0</v>
       </c>
@@ -716,7 +850,9 @@
       </c>
     </row>
     <row r="17" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="2"/>
+      <c r="A17" s="2" t="s">
+        <v>51</v>
+      </c>
       <c r="B17" s="2" t="s">
         <v>0</v>
       </c>
@@ -730,7 +866,9 @@
       </c>
     </row>
     <row r="18" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="2"/>
+      <c r="A18" s="2" t="s">
+        <v>52</v>
+      </c>
       <c r="B18" s="2" t="s">
         <v>0</v>
       </c>
@@ -744,7 +882,9 @@
       </c>
     </row>
     <row r="19" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="2"/>
+      <c r="A19" s="2" t="s">
+        <v>53</v>
+      </c>
       <c r="B19" s="2" t="s">
         <v>0</v>
       </c>
@@ -758,7 +898,9 @@
       </c>
     </row>
     <row r="20" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="2"/>
+      <c r="A20" s="2" t="s">
+        <v>54</v>
+      </c>
       <c r="B20" s="2" t="s">
         <v>0</v>
       </c>
@@ -772,7 +914,9 @@
       </c>
     </row>
     <row r="21" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="2"/>
+      <c r="A21" s="2" t="s">
+        <v>55</v>
+      </c>
       <c r="B21" s="2" t="s">
         <v>0</v>
       </c>
@@ -786,7 +930,9 @@
       </c>
     </row>
     <row r="22" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="2"/>
+      <c r="A22" s="2" t="s">
+        <v>56</v>
+      </c>
       <c r="B22" s="2" t="s">
         <v>0</v>
       </c>
@@ -800,7 +946,9 @@
       </c>
     </row>
     <row r="23" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="2"/>
+      <c r="A23" s="2" t="s">
+        <v>57</v>
+      </c>
       <c r="B23" s="2" t="s">
         <v>0</v>
       </c>
@@ -814,7 +962,9 @@
       </c>
     </row>
     <row r="24" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="2"/>
+      <c r="A24" s="2" t="s">
+        <v>58</v>
+      </c>
       <c r="B24" s="2" t="s">
         <v>0</v>
       </c>
@@ -828,7 +978,9 @@
       </c>
     </row>
     <row r="25" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="2"/>
+      <c r="A25" s="2" t="s">
+        <v>59</v>
+      </c>
       <c r="B25" s="2" t="s">
         <v>0</v>
       </c>
@@ -842,7 +994,9 @@
       </c>
     </row>
     <row r="26" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="2"/>
+      <c r="A26" s="2" t="s">
+        <v>60</v>
+      </c>
       <c r="B26" s="2" t="s">
         <v>0</v>
       </c>
@@ -856,7 +1010,9 @@
       </c>
     </row>
     <row r="27" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="2"/>
+      <c r="A27" s="2" t="s">
+        <v>61</v>
+      </c>
       <c r="B27" s="2" t="s">
         <v>0</v>
       </c>
@@ -870,7 +1026,9 @@
       </c>
     </row>
     <row r="28" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="2"/>
+      <c r="A28" s="2" t="s">
+        <v>62</v>
+      </c>
       <c r="B28" s="2" t="s">
         <v>0</v>
       </c>
@@ -884,7 +1042,9 @@
       </c>
     </row>
     <row r="29" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="2"/>
+      <c r="A29" s="2" t="s">
+        <v>63</v>
+      </c>
       <c r="B29" s="2" t="s">
         <v>0</v>
       </c>
@@ -898,7 +1058,9 @@
       </c>
     </row>
     <row r="30" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="2"/>
+      <c r="A30" s="2" t="s">
+        <v>64</v>
+      </c>
       <c r="B30" s="2" t="s">
         <v>0</v>
       </c>
@@ -912,7 +1074,9 @@
       </c>
     </row>
     <row r="31" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="2"/>
+      <c r="A31" s="2" t="s">
+        <v>65</v>
+      </c>
       <c r="B31" s="2" t="s">
         <v>0</v>
       </c>
@@ -926,7 +1090,9 @@
       </c>
     </row>
     <row r="32" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="2"/>
+      <c r="A32" s="2" t="s">
+        <v>66</v>
+      </c>
       <c r="B32" s="2" t="s">
         <v>0</v>
       </c>
@@ -940,7 +1106,9 @@
       </c>
     </row>
     <row r="33" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="2"/>
+      <c r="A33" s="2" t="s">
+        <v>67</v>
+      </c>
       <c r="B33" s="2" t="s">
         <v>0</v>
       </c>
@@ -954,7 +1122,9 @@
       </c>
     </row>
     <row r="34" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="2"/>
+      <c r="A34" s="2" t="s">
+        <v>68</v>
+      </c>
       <c r="B34" s="2" t="s">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
added WG numbers and other metadata
</commit_message>
<xml_diff>
--- a/publication/part1000/CR_itemshape_1/WG_Number_excel_table.xlsx
+++ b/publication/part1000/CR_itemshape_1/WG_Number_excel_table.xlsx
@@ -134,106 +134,106 @@
     <t>ISO 10303-1816 ed2 model_based_3d_geometrical_dimensioning_and_tolerancing_representation ARM EXPRESS</t>
   </si>
   <si>
-    <t>N1111</t>
-  </si>
-  <si>
-    <t>N1112</t>
-  </si>
-  <si>
-    <t>N1113</t>
-  </si>
-  <si>
-    <t>N1114</t>
-  </si>
-  <si>
-    <t>N1115</t>
-  </si>
-  <si>
-    <t>N1116</t>
-  </si>
-  <si>
-    <t>N1117</t>
-  </si>
-  <si>
-    <t>N1118</t>
-  </si>
-  <si>
-    <t>N1119</t>
-  </si>
-  <si>
-    <t>N1120</t>
-  </si>
-  <si>
-    <t>N1121</t>
-  </si>
-  <si>
-    <t>N1122</t>
-  </si>
-  <si>
-    <t>N1123</t>
-  </si>
-  <si>
-    <t>N1124</t>
-  </si>
-  <si>
-    <t>N1125</t>
-  </si>
-  <si>
-    <t>N1126</t>
-  </si>
-  <si>
-    <t>N1127</t>
-  </si>
-  <si>
-    <t>N1128</t>
-  </si>
-  <si>
-    <t>N1129</t>
-  </si>
-  <si>
-    <t>N1130</t>
-  </si>
-  <si>
-    <t>N1131</t>
-  </si>
-  <si>
-    <t>N1132</t>
-  </si>
-  <si>
-    <t>N1133</t>
-  </si>
-  <si>
-    <t>N1134</t>
-  </si>
-  <si>
-    <t>N1135</t>
-  </si>
-  <si>
-    <t>N1136</t>
-  </si>
-  <si>
-    <t>N1137</t>
-  </si>
-  <si>
-    <t>N1138</t>
-  </si>
-  <si>
-    <t>N1139</t>
-  </si>
-  <si>
-    <t>N1140</t>
-  </si>
-  <si>
-    <t>N1141</t>
-  </si>
-  <si>
-    <t>N1142</t>
-  </si>
-  <si>
-    <t>N1143</t>
-  </si>
-  <si>
-    <t>N1144</t>
+    <t>N9271</t>
+  </si>
+  <si>
+    <t>N9272</t>
+  </si>
+  <si>
+    <t>N9273</t>
+  </si>
+  <si>
+    <t>N9274</t>
+  </si>
+  <si>
+    <t>N9275</t>
+  </si>
+  <si>
+    <t>N9276</t>
+  </si>
+  <si>
+    <t>N9277</t>
+  </si>
+  <si>
+    <t>N9278</t>
+  </si>
+  <si>
+    <t>N9279</t>
+  </si>
+  <si>
+    <t>N9280</t>
+  </si>
+  <si>
+    <t>N9281</t>
+  </si>
+  <si>
+    <t>N9282</t>
+  </si>
+  <si>
+    <t>N9283</t>
+  </si>
+  <si>
+    <t>N9284</t>
+  </si>
+  <si>
+    <t>N9285</t>
+  </si>
+  <si>
+    <t>N9286</t>
+  </si>
+  <si>
+    <t>N9287</t>
+  </si>
+  <si>
+    <t>N9288</t>
+  </si>
+  <si>
+    <t>N9289</t>
+  </si>
+  <si>
+    <t>N9290</t>
+  </si>
+  <si>
+    <t>N9291</t>
+  </si>
+  <si>
+    <t>N9292</t>
+  </si>
+  <si>
+    <t>N9293</t>
+  </si>
+  <si>
+    <t>N9294</t>
+  </si>
+  <si>
+    <t>N9295</t>
+  </si>
+  <si>
+    <t>N9296</t>
+  </si>
+  <si>
+    <t>N9297</t>
+  </si>
+  <si>
+    <t>N9298</t>
+  </si>
+  <si>
+    <t>N9299</t>
+  </si>
+  <si>
+    <t>N9300</t>
+  </si>
+  <si>
+    <t>N9301</t>
+  </si>
+  <si>
+    <t>N9302</t>
+  </si>
+  <si>
+    <t>N9303</t>
+  </si>
+  <si>
+    <t>N9304</t>
   </si>
 </sst>
 </file>
@@ -582,7 +582,7 @@
   <dimension ref="A1:F34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="F2" sqref="F2:F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -606,7 +606,7 @@
         <v>1</v>
       </c>
       <c r="F1" s="4">
-        <v>42658</v>
+        <v>42662</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -622,7 +622,7 @@
         <v>2</v>
       </c>
       <c r="F2" s="4">
-        <v>42658</v>
+        <v>42662</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -638,7 +638,7 @@
         <v>3</v>
       </c>
       <c r="F3" s="4">
-        <v>42658</v>
+        <v>42662</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -654,7 +654,7 @@
         <v>4</v>
       </c>
       <c r="F4" s="4">
-        <v>42658</v>
+        <v>42662</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -670,7 +670,7 @@
         <v>5</v>
       </c>
       <c r="F5" s="4">
-        <v>42658</v>
+        <v>42662</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -686,7 +686,7 @@
         <v>6</v>
       </c>
       <c r="F6" s="4">
-        <v>42658</v>
+        <v>42662</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -702,7 +702,7 @@
         <v>7</v>
       </c>
       <c r="F7" s="4">
-        <v>42658</v>
+        <v>42662</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -718,7 +718,7 @@
         <v>8</v>
       </c>
       <c r="F8" s="4">
-        <v>42658</v>
+        <v>42662</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -734,7 +734,7 @@
         <v>9</v>
       </c>
       <c r="F9" s="4">
-        <v>42658</v>
+        <v>42662</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -750,7 +750,7 @@
         <v>10</v>
       </c>
       <c r="F10" s="4">
-        <v>42658</v>
+        <v>42662</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -766,7 +766,7 @@
         <v>11</v>
       </c>
       <c r="F11" s="4">
-        <v>42658</v>
+        <v>42662</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -782,7 +782,7 @@
         <v>12</v>
       </c>
       <c r="F12" s="4">
-        <v>42658</v>
+        <v>42662</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -798,7 +798,7 @@
         <v>13</v>
       </c>
       <c r="F13" s="4">
-        <v>42658</v>
+        <v>42662</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -814,7 +814,7 @@
         <v>14</v>
       </c>
       <c r="F14" s="4">
-        <v>42658</v>
+        <v>42662</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -830,7 +830,7 @@
         <v>15</v>
       </c>
       <c r="F15" s="4">
-        <v>42658</v>
+        <v>42662</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -846,7 +846,7 @@
         <v>16</v>
       </c>
       <c r="F16" s="4">
-        <v>42658</v>
+        <v>42662</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -862,7 +862,7 @@
         <v>17</v>
       </c>
       <c r="F17" s="4">
-        <v>42658</v>
+        <v>42662</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -878,7 +878,7 @@
         <v>18</v>
       </c>
       <c r="F18" s="4">
-        <v>42658</v>
+        <v>42662</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -894,7 +894,7 @@
         <v>19</v>
       </c>
       <c r="F19" s="4">
-        <v>42658</v>
+        <v>42662</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -910,7 +910,7 @@
         <v>20</v>
       </c>
       <c r="F20" s="4">
-        <v>42658</v>
+        <v>42662</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -926,7 +926,7 @@
         <v>21</v>
       </c>
       <c r="F21" s="4">
-        <v>42658</v>
+        <v>42662</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -942,7 +942,7 @@
         <v>22</v>
       </c>
       <c r="F22" s="4">
-        <v>42658</v>
+        <v>42662</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -958,7 +958,7 @@
         <v>23</v>
       </c>
       <c r="F23" s="4">
-        <v>42658</v>
+        <v>42662</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -974,7 +974,7 @@
         <v>24</v>
       </c>
       <c r="F24" s="4">
-        <v>42658</v>
+        <v>42662</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -990,7 +990,7 @@
         <v>25</v>
       </c>
       <c r="F25" s="4">
-        <v>42658</v>
+        <v>42662</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -1006,7 +1006,7 @@
         <v>26</v>
       </c>
       <c r="F26" s="4">
-        <v>42658</v>
+        <v>42662</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -1022,7 +1022,7 @@
         <v>27</v>
       </c>
       <c r="F27" s="4">
-        <v>42658</v>
+        <v>42662</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -1038,7 +1038,7 @@
         <v>28</v>
       </c>
       <c r="F28" s="4">
-        <v>42658</v>
+        <v>42662</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -1054,7 +1054,7 @@
         <v>29</v>
       </c>
       <c r="F29" s="4">
-        <v>42658</v>
+        <v>42662</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -1070,7 +1070,7 @@
         <v>30</v>
       </c>
       <c r="F30" s="4">
-        <v>42658</v>
+        <v>42662</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -1086,7 +1086,7 @@
         <v>31</v>
       </c>
       <c r="F31" s="4">
-        <v>42658</v>
+        <v>42662</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -1102,7 +1102,7 @@
         <v>32</v>
       </c>
       <c r="F32" s="4">
-        <v>42658</v>
+        <v>42662</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -1118,7 +1118,7 @@
         <v>33</v>
       </c>
       <c r="F33" s="4">
-        <v>42658</v>
+        <v>42662</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -1134,7 +1134,7 @@
         <v>34</v>
       </c>
       <c r="F34" s="4">
-        <v>42658</v>
+        <v>42662</v>
       </c>
     </row>
   </sheetData>

</xml_diff>